<commit_message>
Corrigindo um nome na planilha de exemplo. Atualizando os nomes dos arquivos nos tools.
</commit_message>
<xml_diff>
--- a/docs/example/exemplo-dados.xlsx
+++ b/docs/example/exemplo-dados.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">EDUARDO</t>
   </si>
   <si>
-    <t xml:space="preserve">FERNANDA</t>
+    <t xml:space="preserve">FLÁVIA</t>
   </si>
   <si>
     <t xml:space="preserve">GUSTAVO</t>
@@ -167,7 +167,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>